<commit_message>
Population of vehicles based on vehicle types technology characteristics
</commit_message>
<xml_diff>
--- a/Data/Transport vehicles.xlsx
+++ b/Data/Transport vehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\NEON-Integrated-Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{975B7C45-19B2-4ABF-8BBF-8C04BC482126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14D85DE-D819-4172-8330-BC2BDD7E006E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B4D63B88-AD3C-4344-BC6A-706C49F0643E}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="161">
   <si>
     <t>Bron: CBS</t>
   </si>
@@ -463,9 +462,6 @@
     <t>fuel</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
     <t>avg km per day</t>
   </si>
   <si>
@@ -505,18 +501,6 @@
     <t>https://opendata.cbs.nl/#/CBS/nl/dataset/83703NED/table</t>
   </si>
   <si>
-    <t>Benzine/benzine hybrid/ethanol</t>
-  </si>
-  <si>
-    <t>Diesel/diesel hybrid</t>
-  </si>
-  <si>
-    <t>LPG/ LPG hybrid</t>
-  </si>
-  <si>
-    <t>Full electric/waterstof</t>
-  </si>
-  <si>
     <t>BEV</t>
   </si>
   <si>
@@ -526,46 +510,19 @@
     <t>FCEV</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>Volledig elektrisch (FEV) (x 1 000)</t>
-  </si>
-  <si>
-    <t>Plug-in hybride (PHEV) (x 1 000)</t>
-  </si>
-  <si>
-    <t>7,4</t>
-  </si>
-  <si>
-    <t>36,8</t>
-  </si>
-  <si>
-    <t>76,3</t>
-  </si>
-  <si>
-    <t>13,7</t>
-  </si>
-  <si>
-    <t>95,7</t>
-  </si>
-  <si>
-    <t>21,8</t>
-  </si>
-  <si>
-    <t>97,3</t>
-  </si>
-  <si>
-    <t>44,7</t>
-  </si>
-  <si>
-    <t>93,9</t>
-  </si>
-  <si>
-    <t>106,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RDW</t>
+    <t>https://www.rvo.nl/sites/default/files/2021/03/Elektrisch%20Rijden%20op%20-%20de%20-%20weg%20-%20voertuigen%20en%20laadpunten%20-%20jaaroverzicht%202020.pdf</t>
+  </si>
+  <si>
+    <t>LPG/CNG/Other</t>
+  </si>
+  <si>
+    <t>amount 2017</t>
+  </si>
+  <si>
+    <t>amount 2020</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -4261,10 +4218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245E37B2-C357-4D98-9672-A33F160A89EE}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4272,7 +4229,7 @@
     <col min="1" max="1" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -4280,16 +4237,19 @@
         <v>139</v>
       </c>
       <c r="C1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -4297,16 +4257,19 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>6509025</v>
-      </c>
-      <c r="D2" s="2">
+        <v>7142431</v>
+      </c>
+      <c r="D2">
+        <v>7655565</v>
+      </c>
+      <c r="E2" s="2">
         <v>12588.584130267225</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>34.489271589773217</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -4314,746 +4277,614 @@
         <v>75</v>
       </c>
       <c r="C3">
-        <v>1314225</v>
-      </c>
-      <c r="D3" s="2">
+        <v>1406856</v>
+      </c>
+      <c r="D3">
+        <v>1161676</v>
+      </c>
+      <c r="E3" s="2">
         <v>12588.584130267225</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>34.489271589773217</v>
       </c>
-      <c r="I3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K3">
-        <v>10748</v>
-      </c>
-      <c r="L3">
-        <v>7340554</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="C4">
-        <v>143542</v>
-      </c>
-      <c r="D4" s="2">
+        <v>166100</v>
+      </c>
+      <c r="D4">
+        <v>137498</v>
+      </c>
+      <c r="E4" s="2">
         <v>12588.584130267225</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>34.489271589773217</v>
       </c>
-      <c r="I4" t="s">
-        <v>155</v>
-      </c>
-      <c r="J4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K4">
-        <v>23361</v>
-      </c>
-      <c r="L4">
-        <v>1518101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C5">
-        <v>245427</v>
-      </c>
-      <c r="D5" s="2">
+        <v>21136</v>
+      </c>
+      <c r="D5">
+        <v>182486</v>
+      </c>
+      <c r="E5" s="2">
         <v>12588.584130267225</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>34.489271589773217</v>
       </c>
-      <c r="I5" t="s">
-        <v>156</v>
-      </c>
-      <c r="J5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5">
-        <v>15483</v>
-      </c>
-      <c r="L5">
-        <v>155943</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
       <c r="B6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="C6">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>390</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12588.584130267225</v>
+      </c>
+      <c r="F6" s="2">
+        <v>34.489271589773217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
       <c r="B7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="C7">
+        <v>98773</v>
+      </c>
+      <c r="D7">
+        <v>109754</v>
+      </c>
+      <c r="E7" s="2">
+        <v>12588.584130267225</v>
+      </c>
+      <c r="F7" s="2">
+        <v>34.489271589773217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>7901</v>
-      </c>
-      <c r="D8" s="2">
-        <v>12588.584130267225</v>
+        <v>26134</v>
       </c>
       <c r="E8" s="2">
-        <v>34.489271589773217</v>
-      </c>
-      <c r="I8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J8" t="s">
-        <v>110</v>
-      </c>
-      <c r="K8">
-        <v>15679</v>
-      </c>
-      <c r="L8">
-        <v>21735</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>19831.181564848612</v>
+      </c>
+      <c r="F8" s="2">
+        <v>54.332004287256467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C9">
-        <v>2854</v>
-      </c>
-      <c r="D9" s="2">
-        <v>12588.584130267225</v>
+        <v>806254</v>
       </c>
       <c r="E9" s="2">
-        <v>34.489271589773217</v>
-      </c>
-      <c r="I9" t="s">
-        <v>151</v>
-      </c>
-      <c r="J9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K9">
-        <v>26278</v>
-      </c>
-      <c r="L9">
-        <v>102173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>19831.181564848612</v>
+      </c>
+      <c r="F9" s="2">
+        <v>54.332004287256467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C10">
-        <v>26134</v>
-      </c>
-      <c r="D10" s="2">
+        <v>15720</v>
+      </c>
+      <c r="E10" s="2">
         <v>19831.181564848612</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>54.332004287256467</v>
       </c>
-      <c r="I10" t="s">
-        <v>152</v>
-      </c>
-      <c r="J10" t="s">
-        <v>110</v>
-      </c>
-      <c r="K10">
-        <v>23492</v>
-      </c>
-      <c r="L10">
-        <v>9698</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C11">
-        <v>806254</v>
-      </c>
-      <c r="D11" s="2">
+        <v>1519</v>
+      </c>
+      <c r="E11" s="2">
         <v>19831.181564848612</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>54.332004287256467</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C12">
-        <v>15720</v>
-      </c>
-      <c r="D12" s="2">
+        <v>2992</v>
+      </c>
+      <c r="E12" s="2">
         <v>19831.181564848612</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>54.332004287256467</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C13">
-        <v>1519</v>
-      </c>
-      <c r="D13" s="2">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
         <v>19831.181564848612</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>54.332004287256467</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>2992</v>
-      </c>
-      <c r="D14" s="2">
-        <v>19831.181564848612</v>
+        <v>870</v>
       </c>
       <c r="E14" s="2">
-        <v>54.332004287256467</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>33998.873783283721</v>
+      </c>
+      <c r="F14" s="2">
+        <v>93.147599406256774</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2">
-        <v>19831.181564848612</v>
+        <v>60660</v>
       </c>
       <c r="E15" s="2">
-        <v>54.332004287256467</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>33998.873783283721</v>
+      </c>
+      <c r="F15" s="2">
+        <v>93.147599406256774</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>120</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C16">
-        <v>870</v>
-      </c>
-      <c r="D16" s="2">
+        <v>292</v>
+      </c>
+      <c r="E16" s="2">
         <v>33998.873783283721</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>93.147599406256774</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C17">
-        <v>60660</v>
-      </c>
-      <c r="D17" s="2">
+        <v>104</v>
+      </c>
+      <c r="E17" s="2">
         <v>33998.873783283721</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>93.147599406256774</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C18">
-        <v>292</v>
-      </c>
-      <c r="D18" s="2">
+        <v>204</v>
+      </c>
+      <c r="E18" s="2">
         <v>33998.873783283721</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>93.147599406256774</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C19">
-        <v>104</v>
-      </c>
-      <c r="D19" s="2">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2">
         <v>33998.873783283721</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>93.147599406256774</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>204</v>
-      </c>
-      <c r="D20" s="2">
-        <v>33998.873783283721</v>
+        <v>28</v>
       </c>
       <c r="E20" s="2">
-        <v>93.147599406256774</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>60029.911881214801</v>
+      </c>
+      <c r="F20" s="2">
+        <v>164.46551200332823</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C21">
-        <v>25</v>
-      </c>
-      <c r="D21" s="2">
-        <v>33998.873783283721</v>
+        <v>73794</v>
       </c>
       <c r="E21" s="2">
-        <v>93.147599406256774</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+        <v>60029.911881214801</v>
+      </c>
+      <c r="F21" s="2">
+        <v>164.46551200332823</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>121</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C22">
-        <v>28</v>
-      </c>
-      <c r="D22" s="2">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
         <v>60029.911881214801</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>164.46551200332823</v>
       </c>
-      <c r="L22" t="s">
-        <v>161</v>
-      </c>
-      <c r="M22" t="s">
-        <v>162</v>
-      </c>
-      <c r="N22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C23">
-        <v>73794</v>
-      </c>
-      <c r="D23" s="2">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2">
         <v>60029.911881214801</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>164.46551200332823</v>
       </c>
-      <c r="L23">
-        <v>2015</v>
-      </c>
-      <c r="M23" t="s">
-        <v>164</v>
-      </c>
-      <c r="N23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C24">
-        <v>20</v>
-      </c>
-      <c r="D24" s="2">
+        <v>116</v>
+      </c>
+      <c r="E24" s="2">
         <v>60029.911881214801</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>164.46551200332823</v>
       </c>
-      <c r="L24">
-        <v>2016</v>
-      </c>
-      <c r="M24">
-        <v>10</v>
-      </c>
-      <c r="N24" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>121</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C25">
-        <v>8</v>
-      </c>
-      <c r="D25" s="2">
+        <v>252</v>
+      </c>
+      <c r="E25" s="2">
         <v>60029.911881214801</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>164.46551200332823</v>
       </c>
-      <c r="L25">
-        <v>2017</v>
-      </c>
-      <c r="M25" t="s">
-        <v>167</v>
-      </c>
-      <c r="N25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>116</v>
-      </c>
-      <c r="D26" s="2">
-        <v>60029.911881214801</v>
+        <v>2647</v>
       </c>
       <c r="E26" s="2">
-        <v>164.46551200332823</v>
-      </c>
-      <c r="L26">
-        <v>2018</v>
-      </c>
-      <c r="M26" t="s">
-        <v>169</v>
-      </c>
-      <c r="N26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>6503.1698365031698</v>
+      </c>
+      <c r="F26" s="2">
+        <v>17.816903661652521</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C27">
-        <v>252</v>
-      </c>
-      <c r="D27" s="2">
-        <v>60029.911881214801</v>
+        <v>55449</v>
       </c>
       <c r="E27" s="2">
-        <v>164.46551200332823</v>
-      </c>
-      <c r="L27">
-        <v>2019</v>
-      </c>
-      <c r="M27" t="s">
-        <v>171</v>
-      </c>
-      <c r="N27" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+        <v>6503.1698365031698</v>
+      </c>
+      <c r="F27" s="2">
+        <v>17.816903661652521</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>135</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C28">
-        <v>2647</v>
-      </c>
-      <c r="D28" s="2">
+        <v>1659</v>
+      </c>
+      <c r="E28" s="2">
         <v>6503.1698365031698</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>17.816903661652521</v>
       </c>
-      <c r="L28">
-        <v>2020</v>
-      </c>
-      <c r="M28" t="s">
-        <v>173</v>
-      </c>
-      <c r="N28">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C29">
-        <v>55449</v>
-      </c>
-      <c r="D29" s="2">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
         <v>6503.1698365031698</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>17.816903661652521</v>
       </c>
-      <c r="L29" t="s">
-        <v>0</v>
-      </c>
-      <c r="M29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C30">
-        <v>1659</v>
-      </c>
-      <c r="D30" s="2">
+        <v>169</v>
+      </c>
+      <c r="E30" s="2">
         <v>6503.1698365031698</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <v>17.816903661652521</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C31">
-        <v>10</v>
-      </c>
-      <c r="D31" s="2">
+        <v>6</v>
+      </c>
+      <c r="E31" s="2">
         <v>6503.1698365031698</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>17.816903661652521</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>169</v>
-      </c>
-      <c r="D32" s="2">
-        <v>6503.1698365031698</v>
+        <v>25</v>
       </c>
       <c r="E32" s="2">
-        <v>17.816903661652521</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66636.122989207899</v>
+      </c>
+      <c r="F32" s="2">
+        <v>182.56472051837781</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2">
-        <v>6503.1698365031698</v>
+        <v>8945</v>
       </c>
       <c r="E33" s="2">
-        <v>17.816903661652521</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66636.122989207899</v>
+      </c>
+      <c r="F33" s="2">
+        <v>182.56472051837781</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>136</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C34">
-        <v>25</v>
-      </c>
-      <c r="D34" s="2">
+        <v>5</v>
+      </c>
+      <c r="E34" s="2">
         <v>66636.122989207899</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
         <v>182.56472051837781</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C35">
-        <v>8945</v>
-      </c>
-      <c r="D35" s="2">
+        <v>191</v>
+      </c>
+      <c r="E35" s="2">
         <v>66636.122989207899</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>182.56472051837781</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C36">
-        <v>5</v>
-      </c>
-      <c r="D36" s="2">
+        <v>656</v>
+      </c>
+      <c r="E36" s="2">
         <v>66636.122989207899</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <v>182.56472051837781</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>136</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C37">
-        <v>191</v>
-      </c>
-      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
         <v>66636.122989207899</v>
       </c>
-      <c r="E37" s="2">
+      <c r="F37" s="2">
         <v>182.56472051837781</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>136</v>
-      </c>
-      <c r="B38" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38">
-        <v>656</v>
-      </c>
-      <c r="D38" s="2">
-        <v>66636.122989207899</v>
-      </c>
-      <c r="E38" s="2">
-        <v>182.56472051837781</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39" s="2">
-        <v>66636.122989207899</v>
-      </c>
-      <c r="E39" s="2">
-        <v>182.56472051837781</v>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5921,7 +5752,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5929,7 +5760,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
         <v>114</v>
@@ -5948,13 +5779,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
         <v>144</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>146</v>
       </c>
       <c r="D6" t="s">
         <v>66</v>
@@ -5976,7 +5807,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
         <v>110</v>
@@ -5990,7 +5821,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
         <v>110</v>
@@ -6004,7 +5835,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B10" t="s">
         <v>110</v>
@@ -6018,7 +5849,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
         <v>110</v>
@@ -6032,7 +5863,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
         <v>110</v>
@@ -6046,7 +5877,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
         <v>110</v>
@@ -6065,7 +5896,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>